<commit_message>
- Make the initial pose of robot randomized
</commit_message>
<xml_diff>
--- a/mazeLib/maze10.xlsx
+++ b/mazeLib/maze10.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Odrive\1.Main_GoogleDrive\Github\EE817_RobotNavigation\mazeLib\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="75" windowWidth="20340" windowHeight="7935"/>
   </bookViews>
@@ -16,8 +21,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -30,6 +35,12 @@
       <name val="Czcionka tekstu podstawowego"/>
       <family val="2"/>
       <charset val="238"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="돋움"/>
+      <family val="3"/>
+      <charset val="129"/>
     </font>
   </fonts>
   <fills count="7">
@@ -190,17 +201,25 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
   <a:themeElements>
-    <a:clrScheme name="Pakiet Office">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -238,9 +257,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Pakiet Office">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -272,9 +291,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -306,9 +326,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Pakiet Office">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -481,11 +502,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CY100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="CZ63" sqref="CZ63"/>
+    <sheetView tabSelected="1" topLeftCell="W66" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="CP95" sqref="CP95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -27373,7 +27394,7 @@
         <v>0</v>
       </c>
       <c r="CU89" s="24">
-        <v>502</v>
+        <v>0</v>
       </c>
       <c r="CV89" s="13">
         <v>0</v>
@@ -30029,7 +30050,7 @@
         <v>0</v>
       </c>
       <c r="BZ98" s="24">
-        <v>501</v>
+        <v>0</v>
       </c>
       <c r="CA98" s="8">
         <v>101</v>
@@ -30703,31 +30724,34 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>